<commit_message>
Check the same accuracy
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -69,7 +72,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Results for the new model new HKG
Do the results, but I have to solve the problem with the MatchComparisonResults porque me da error y no se porque
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -90,7 +93,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Global for the new HKL
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -96,7 +99,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Compare the 2 HKLists
compare the percentage of the similarity between both housekeeping gene lists, the result is that 74%
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -99,7 +105,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Changes for new model and new dataset
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -120,247 +123,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>50.070323488045013</v>
+        <v>70.652173913043484</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>49.929676511954995</v>
+        <v>70.380434782608688</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>50.210970464135016</v>
+        <v>70.380434782608688</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>49.507735583684955</v>
+        <v>70.108695652173907</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>49.507735583684955</v>
+        <v>69.83695652173914</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>49.367088607594937</v>
+        <v>70.108695652173907</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>51.61744022503516</v>
+        <v>71.739130434782609</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>51.336146272855132</v>
+        <v>72.282608695652172</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>51.61744022503516</v>
+        <v>72.554347826086953</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>51.898734177215189</v>
+        <v>72.282608695652172</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>50.351617440225041</v>
+        <v>70.652173913043484</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>50.914205344585092</v>
+        <v>71.739130434782609</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>51.758087201125178</v>
+        <v>72.554347826086953</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>51.61744022503516</v>
+        <v>72.554347826086953</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>52.180028129395218</v>
+        <v>72.554347826086953</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>50.492264416315045</v>
+        <v>71.467391304347828</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>50.773558368495074</v>
+        <v>71.739130434782609</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>49.929676511954995</v>
+        <v>71.739130434782609</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>50.632911392405063</v>
+        <v>71.739130434782609</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>51.054852320675103</v>
+        <v>72.282608695652172</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>50.914205344585092</v>
+        <v>72.554347826086953</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>48.804500703234879</v>
+        <v>69.021739130434781</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>48.38255977496484</v>
+        <v>70.380434782608688</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>48.52320675105485</v>
+        <v>69.565217391304344</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>50.632911392405063</v>
+        <v>71.195652173913047</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>50.914205344585092</v>
+        <v>71.739130434782609</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>51.195499296765121</v>
+        <v>72.282608695652172</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>52.180028129395218</v>
+        <v>73.369565217391312</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>51.47679324894515</v>
+        <v>73.097826086956516</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>51.758087201125178</v>
+        <v>73.097826086956516</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>48.945147679324897</v>
+        <v>69.565217391304344</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>49.367088607594937</v>
+        <v>69.83695652173914</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>49.789029535864984</v>
+        <v>70.923913043478265</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>50.632911392405063</v>
+        <v>70.652173913043484</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>50.070323488045013</v>
+        <v>70.108695652173907</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>53.586497890295362</v>
+        <v>71.195652173913047</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>48.945147679324897</v>
+        <v>69.021739130434781</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>49.929676511954995</v>
+        <v>69.021739130434781</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>49.929676511954995</v>
+        <v>69.565217391304344</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>51.47679324894515</v>
+        <v>72.282608695652172</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>51.61744022503516</v>
+        <v>72.282608695652172</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>51.758087201125178</v>
+        <v>72.282608695652172</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>51.61744022503516</v>
+        <v>71.739130434782609</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>50.351617440225041</v>
+        <v>69.565217391304344</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>50.351617440225041</v>
+        <v>70.380434782608688</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>49.226441631504926</v>
+        <v>69.565217391304344</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>51.898734177215189</v>
+        <v>70.380434782608688</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>50.632911392405063</v>
+        <v>69.83695652173914</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Better descripton  of localT2 ls
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -123,247 +126,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>70.652173913043484</v>
+        <v>50.070323488045013</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>70.380434782608688</v>
+        <v>49.929676511954995</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>70.380434782608688</v>
+        <v>50.210970464135016</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>70.108695652173907</v>
+        <v>49.507735583684955</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>69.83695652173914</v>
+        <v>49.507735583684955</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>70.108695652173907</v>
+        <v>49.367088607594937</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>71.739130434782609</v>
+        <v>51.61744022503516</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>72.282608695652172</v>
+        <v>51.336146272855132</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>72.554347826086953</v>
+        <v>51.61744022503516</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>72.282608695652172</v>
+        <v>51.898734177215189</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>70.652173913043484</v>
+        <v>50.351617440225041</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>71.739130434782609</v>
+        <v>50.914205344585092</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>72.554347826086953</v>
+        <v>51.758087201125178</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>72.554347826086953</v>
+        <v>51.61744022503516</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>72.554347826086953</v>
+        <v>52.180028129395218</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>71.467391304347828</v>
+        <v>50.492264416315045</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>71.739130434782609</v>
+        <v>50.773558368495074</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>71.739130434782609</v>
+        <v>49.929676511954995</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>71.739130434782609</v>
+        <v>50.632911392405063</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>72.282608695652172</v>
+        <v>51.054852320675103</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>72.554347826086953</v>
+        <v>50.914205344585092</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>69.021739130434781</v>
+        <v>48.804500703234879</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>70.380434782608688</v>
+        <v>48.38255977496484</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>69.565217391304344</v>
+        <v>48.52320675105485</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>71.195652173913047</v>
+        <v>50.632911392405063</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>71.739130434782609</v>
+        <v>50.914205344585092</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>72.282608695652172</v>
+        <v>51.195499296765121</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>73.369565217391312</v>
+        <v>52.180028129395218</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>73.097826086956516</v>
+        <v>51.47679324894515</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>73.097826086956516</v>
+        <v>51.758087201125178</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>69.565217391304344</v>
+        <v>48.945147679324897</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>69.83695652173914</v>
+        <v>49.367088607594937</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>70.923913043478265</v>
+        <v>49.789029535864984</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>70.652173913043484</v>
+        <v>50.632911392405063</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>70.108695652173907</v>
+        <v>50.070323488045013</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>71.195652173913047</v>
+        <v>53.586497890295362</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>69.021739130434781</v>
+        <v>48.945147679324897</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>69.021739130434781</v>
+        <v>49.929676511954995</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>69.565217391304344</v>
+        <v>49.929676511954995</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>72.282608695652172</v>
+        <v>51.47679324894515</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>72.282608695652172</v>
+        <v>51.61744022503516</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>72.282608695652172</v>
+        <v>51.758087201125178</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>71.739130434782609</v>
+        <v>51.61744022503516</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>69.565217391304344</v>
+        <v>50.351617440225041</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>70.380434782608688</v>
+        <v>50.351617440225041</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>69.565217391304344</v>
+        <v>49.226441631504926</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>70.380434782608688</v>
+        <v>51.898734177215189</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>69.83695652173914</v>
+        <v>50.632911392405063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New reaction for global thresholding
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -129,7 +132,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Global test(not finsish it gives me a shit)
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -132,7 +138,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
New approach for global, final
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -144,7 +153,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
New method GT, finished
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -153,7 +156,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Final code for Global
Needs to improe and check some htings, and put it nicely
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -156,247 +174,247 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>50.070323488045013</v>
+        <v>52.072072072072075</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>49.929676511954995</v>
+        <v>51.711711711711715</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>50.210970464135016</v>
+        <v>51.891891891891895</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>49.507735583684955</v>
+        <v>51.531531531531527</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>49.507735583684955</v>
+        <v>51.351351351351347</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>49.367088607594937</v>
+        <v>51.531531531531527</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>51.61744022503516</v>
+        <v>53.693693693693689</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>51.336146272855132</v>
+        <v>53.153153153153156</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>51.61744022503516</v>
+        <v>53.153153153153156</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>51.898734177215189</v>
+        <v>53.333333333333336</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>50.351617440225041</v>
+        <v>52.432432432432428</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>50.914205344585092</v>
+        <v>52.792792792792795</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>51.758087201125178</v>
+        <v>54.054054054054056</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>51.61744022503516</v>
+        <v>54.054054054054056</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>52.180028129395218</v>
+        <v>53.873873873873876</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>50.492264416315045</v>
+        <v>52.612612612612608</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>50.773558368495074</v>
+        <v>52.792792792792795</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>49.929676511954995</v>
+        <v>52.252252252252248</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>50.632911392405063</v>
+        <v>52.612612612612608</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>51.054852320675103</v>
+        <v>52.612612612612608</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>50.914205344585092</v>
+        <v>52.972972972972975</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>48.804500703234879</v>
+        <v>50.810810810810814</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>48.38255977496484</v>
+        <v>49.909909909909913</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>48.52320675105485</v>
+        <v>50.990990990990994</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>50.632911392405063</v>
+        <v>52.792792792792795</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>50.914205344585092</v>
+        <v>52.612612612612608</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>51.195499296765121</v>
+        <v>53.513513513513509</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>52.180028129395218</v>
+        <v>54.414414414414416</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>51.47679324894515</v>
+        <v>53.873873873873876</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>51.758087201125178</v>
+        <v>54.234234234234236</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>48.945147679324897</v>
+        <v>50.450450450450447</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>49.367088607594937</v>
+        <v>51.531531531531527</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>49.789029535864984</v>
+        <v>51.711711711711715</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>50.632911392405063</v>
+        <v>52.072072072072075</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>50.070323488045013</v>
+        <v>51.531531531531527</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>53.586497890295362</v>
+        <v>56.216216216216218</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>48.945147679324897</v>
+        <v>50.810810810810814</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>49.929676511954995</v>
+        <v>51.711711711711715</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>49.929676511954995</v>
+        <v>51.171171171171167</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>51.47679324894515</v>
+        <v>52.612612612612608</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>51.61744022503516</v>
+        <v>53.153153153153156</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>51.758087201125178</v>
+        <v>53.873873873873876</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>51.61744022503516</v>
+        <v>53.333333333333336</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>50.351617440225041</v>
+        <v>52.252252252252248</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>50.351617440225041</v>
+        <v>52.432432432432428</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>49.226441631504926</v>
+        <v>51.531531531531527</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>51.898734177215189</v>
+        <v>54.054054054054056</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>50.632911392405063</v>
+        <v>52.972972972972975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in global thresholding
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -174,7 +186,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
'OR' 'AND' rules analyzed
Percentage of or and rules for each one
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -189,7 +192,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Create the function to calcultae how many OR, AND rules
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -201,7 +204,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
Plots for GlobalThrehsolding and gini coefficient between samples and genes
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -204,7 +207,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
OR and AND rules
totalRulesWithBoth = countRulesWithBothOperators(model.grRules);
fprintf('Total de reglas que contienen AND y OR: %d\n', totalRulesWithBoth);
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -213,7 +216,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
New check of the normalization
Code to check the normalization with different values
</commit_message>
<xml_diff>
--- a/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
+++ b/Thresholding/Global_Threshold/HK_G_acc_G.xlsx
@@ -13,7 +13,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
+  <si>
+    <t>HK_G_acc_G</t>
+  </si>
   <si>
     <t>HK_G_acc_G</t>
   </si>
@@ -225,7 +231,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">

</xml_diff>